<commit_message>
small edit to the player stat table xlsx document
</commit_message>
<xml_diff>
--- a/FLC_isometricGame_statTable_v001.xlsx
+++ b/FLC_isometricGame_statTable_v001.xlsx
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +162,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,19 +190,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +508,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,92 +532,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>0</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>160</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>50</v>
       </c>
       <c r="E3">
@@ -645,24 +653,24 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="5">
         <v>5</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>120</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>200</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <f>FLOOR(D3*1.25,1)</f>
         <v>62</v>
       </c>
@@ -699,25 +707,25 @@
       <c r="O4">
         <v>5</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="5">
         <v>5</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <f>FLOOR(B4*1.5,1)</f>
         <v>180</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>250</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <f t="shared" ref="D5:D12" si="0">FLOOR(D4*1.25,1)</f>
         <v>77</v>
       </c>
@@ -754,25 +762,25 @@
       <c r="O5">
         <v>10</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="5">
         <v>5</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <f t="shared" ref="B6:B12" si="1">FLOOR(B5*1.5,1)</f>
         <v>270</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>300</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
@@ -809,25 +817,25 @@
       <c r="O6">
         <v>15</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="5">
         <v>5</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="5">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <f t="shared" si="1"/>
         <v>405</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>450</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -864,25 +872,25 @@
       <c r="O7">
         <v>20</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="5">
         <v>6</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="5">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <f t="shared" si="1"/>
         <v>607</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>550</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -919,25 +927,25 @@
       <c r="O8">
         <v>25</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="5">
         <v>7</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="5">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <f t="shared" si="1"/>
         <v>910</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="5">
         <v>700</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <f t="shared" si="0"/>
         <v>187</v>
       </c>
@@ -974,25 +982,25 @@
       <c r="O9">
         <v>30</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="5">
         <v>8</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="5">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <f t="shared" si="1"/>
         <v>1365</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="5">
         <v>900</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <f t="shared" si="0"/>
         <v>233</v>
       </c>
@@ -1029,25 +1037,25 @@
       <c r="O10">
         <v>35</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="5">
         <v>9</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="5">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <f t="shared" si="1"/>
         <v>2047</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>1120</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <f t="shared" si="0"/>
         <v>291</v>
       </c>
@@ -1084,25 +1092,25 @@
       <c r="O11">
         <v>40</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="5">
         <v>10</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="5">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <f t="shared" si="1"/>
         <v>3070</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>1400</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <f t="shared" si="0"/>
         <v>363</v>
       </c>
@@ -1139,34 +1147,34 @@
       <c r="O12">
         <v>45</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="5">
         <v>15</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="5">
         <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P13" s="6">
+      <c r="P13" s="4">
         <f>SUM(P3:P12)</f>
         <v>75</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="4">
         <f>SUM(Q3:Q12)</f>
         <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
stat table conditioning column adjustment
</commit_message>
<xml_diff>
--- a/FLC_isometricGame_statTable_v001.xlsx
+++ b/FLC_isometricGame_statTable_v001.xlsx
@@ -197,13 +197,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +508,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,27 +532,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -617,7 +617,7 @@
       <c r="C3" s="5">
         <v>160</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>50</v>
       </c>
       <c r="E3">
@@ -670,7 +670,7 @@
       <c r="C4" s="5">
         <v>200</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <f>FLOOR(D3*1.25,1)</f>
         <v>62</v>
       </c>
@@ -684,7 +684,7 @@
         <v>10</v>
       </c>
       <c r="H4">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I4">
         <v>5</v>
@@ -725,7 +725,7 @@
       <c r="C5" s="5">
         <v>250</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <f t="shared" ref="D5:D12" si="0">FLOOR(D4*1.25,1)</f>
         <v>77</v>
       </c>
@@ -739,7 +739,8 @@
         <v>12</v>
       </c>
       <c r="H5">
-        <v>31</v>
+        <f>ROUND(1.3125*H4,0)</f>
+        <v>30</v>
       </c>
       <c r="I5">
         <v>10</v>
@@ -780,7 +781,7 @@
       <c r="C6" s="5">
         <v>300</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <f t="shared" si="0"/>
         <v>96</v>
       </c>
@@ -794,7 +795,8 @@
         <v>14</v>
       </c>
       <c r="H6">
-        <v>42</v>
+        <f t="shared" ref="H6:H12" si="2">ROUND(1.3125*H5,0)</f>
+        <v>39</v>
       </c>
       <c r="I6">
         <v>15</v>
@@ -835,7 +837,7 @@
       <c r="C7" s="5">
         <v>450</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -849,7 +851,8 @@
         <v>16</v>
       </c>
       <c r="H7">
-        <v>56</v>
+        <f t="shared" si="2"/>
+        <v>51</v>
       </c>
       <c r="I7">
         <v>20</v>
@@ -890,7 +893,7 @@
       <c r="C8" s="5">
         <v>550</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -904,7 +907,8 @@
         <v>20</v>
       </c>
       <c r="H8">
-        <v>75</v>
+        <f t="shared" si="2"/>
+        <v>67</v>
       </c>
       <c r="I8">
         <v>25</v>
@@ -945,7 +949,7 @@
       <c r="C9" s="5">
         <v>700</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <f t="shared" si="0"/>
         <v>187</v>
       </c>
@@ -959,7 +963,8 @@
         <v>24</v>
       </c>
       <c r="H9">
-        <v>101</v>
+        <f t="shared" si="2"/>
+        <v>88</v>
       </c>
       <c r="I9">
         <v>30</v>
@@ -1000,7 +1005,7 @@
       <c r="C10" s="5">
         <v>900</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <f t="shared" si="0"/>
         <v>233</v>
       </c>
@@ -1014,7 +1019,8 @@
         <v>30</v>
       </c>
       <c r="H10">
-        <v>134</v>
+        <f t="shared" si="2"/>
+        <v>116</v>
       </c>
       <c r="I10">
         <v>35</v>
@@ -1055,7 +1061,7 @@
       <c r="C11" s="5">
         <v>1120</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <f t="shared" si="0"/>
         <v>291</v>
       </c>
@@ -1069,7 +1075,8 @@
         <v>36</v>
       </c>
       <c r="H11">
-        <v>179</v>
+        <f>ROUND(1.3125*H10,0)</f>
+        <v>152</v>
       </c>
       <c r="I11">
         <v>40</v>
@@ -1110,7 +1117,7 @@
       <c r="C12" s="5">
         <v>1400</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <f t="shared" si="0"/>
         <v>363</v>
       </c>
@@ -1124,7 +1131,8 @@
         <v>45</v>
       </c>
       <c r="H12">
-        <v>239</v>
+        <f t="shared" si="2"/>
+        <v>200</v>
       </c>
       <c r="I12">
         <v>45</v>
@@ -1165,16 +1173,16 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1217,11 +1225,11 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:B35" si="2">FLOOR(C17*1.25,1)</f>
+        <f t="shared" ref="B18:B35" si="3">FLOOR(C17*1.25,1)</f>
         <v>120</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:C35" si="3">FLOOR(B18*1.25,1)</f>
+        <f t="shared" ref="C18:C35" si="4">FLOOR(B18*1.25,1)</f>
         <v>150</v>
       </c>
     </row>
@@ -1230,11 +1238,11 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>187</v>
       </c>
       <c r="C19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>233</v>
       </c>
     </row>
@@ -1243,11 +1251,11 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>291</v>
       </c>
       <c r="C20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>363</v>
       </c>
     </row>
@@ -1256,11 +1264,11 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>453</v>
       </c>
       <c r="C21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>566</v>
       </c>
     </row>
@@ -1269,11 +1277,11 @@
         <v>7</v>
       </c>
       <c r="B22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>707</v>
       </c>
       <c r="C22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>883</v>
       </c>
     </row>
@@ -1282,11 +1290,11 @@
         <v>8</v>
       </c>
       <c r="B23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1103</v>
       </c>
       <c r="C23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1378</v>
       </c>
     </row>
@@ -1295,11 +1303,11 @@
         <v>9</v>
       </c>
       <c r="B24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1722</v>
       </c>
       <c r="C24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2152</v>
       </c>
     </row>
@@ -1308,11 +1316,11 @@
         <v>10</v>
       </c>
       <c r="B25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2690</v>
       </c>
       <c r="C25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3362</v>
       </c>
     </row>
@@ -1321,11 +1329,11 @@
         <v>11</v>
       </c>
       <c r="B26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4202</v>
       </c>
       <c r="C26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5252</v>
       </c>
     </row>
@@ -1334,11 +1342,11 @@
         <v>12</v>
       </c>
       <c r="B27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6565</v>
       </c>
       <c r="C27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8206</v>
       </c>
     </row>
@@ -1347,11 +1355,11 @@
         <v>13</v>
       </c>
       <c r="B28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10257</v>
       </c>
       <c r="C28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12821</v>
       </c>
     </row>
@@ -1360,11 +1368,11 @@
         <v>14</v>
       </c>
       <c r="B29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16026</v>
       </c>
       <c r="C29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20032</v>
       </c>
     </row>
@@ -1373,11 +1381,11 @@
         <v>15</v>
       </c>
       <c r="B30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25040</v>
       </c>
       <c r="C30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>31300</v>
       </c>
     </row>
@@ -1386,11 +1394,11 @@
         <v>16</v>
       </c>
       <c r="B31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>39125</v>
       </c>
       <c r="C31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48906</v>
       </c>
     </row>
@@ -1399,11 +1407,11 @@
         <v>17</v>
       </c>
       <c r="B32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>61132</v>
       </c>
       <c r="C32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76415</v>
       </c>
     </row>
@@ -1412,11 +1420,11 @@
         <v>18</v>
       </c>
       <c r="B33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>95518</v>
       </c>
       <c r="C33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>119397</v>
       </c>
     </row>
@@ -1425,11 +1433,11 @@
         <v>19</v>
       </c>
       <c r="B34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>149246</v>
       </c>
       <c r="C34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>186557</v>
       </c>
     </row>
@@ -1438,11 +1446,11 @@
         <v>20</v>
       </c>
       <c r="B35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>233196</v>
       </c>
       <c r="C35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>291495</v>
       </c>
     </row>

</xml_diff>